<commit_message>
Added Wordnik and improved eval. script for time consumption
</commit_message>
<xml_diff>
--- a/src/output_detections_highlighting_without_annotations.xlsx
+++ b/src/output_detections_highlighting_without_annotations.xlsx
@@ -8,15 +8,18 @@
   </bookViews>
   <sheets>
     <sheet name="Only US-Result sheet " sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Only US-Result" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Only US-False Pos. Neg." sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Only US-True Pos." sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Only US-Result" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Only US-False Pos. Neg." sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Only US-True Pos." sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="TimeConsupNoAnn" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Only US-Result sheet '!$A$1:$O$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Only US-Result'!$A$1:$O$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Only US-False Pos. Neg.'!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Only US-True Pos.'!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Only US-Result'!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Only US-False Pos. Neg.'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Only US-True Pos.'!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'TimeConsupNoAnn'!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -805,6 +808,61 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>total_time_3_5</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>avg_time_3_5</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>total_time_4</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>avg_time_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1158,7 +1216,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1371,7 +1429,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1508,4 +1566,125 @@
   <autoFilter ref="A1:J1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13.5" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Version</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Groups</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Total Time</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Avg Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>v3.5</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>All sets</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>1005</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>v4</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>All sets</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>v3.5</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>00_#G03#</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>1005</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>v4</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>00_#G03#</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commit of the day
</commit_message>
<xml_diff>
--- a/src/output_detections_highlighting_without_annotations.xlsx
+++ b/src/output_detections_highlighting_without_annotations.xlsx
@@ -7,19 +7,16 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Only US-Result sheet " sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Only US-Result" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Only US-False Pos. Neg." sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Only US-True Pos." sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="TimeConsupNoAnn" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Only US-Result" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Only US-False Pos. Neg." sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Only US-True Pos." sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Time Consup." sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Only US-Result sheet '!$A$1:$O$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Only US-Result'!$A$1:$O$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Only US-False Pos. Neg.'!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Only US-True Pos.'!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'TimeConsupNoAnn'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Only US-Result'!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Only US-False Pos. Neg.'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Only US-True Pos.'!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Time Consup.'!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -555,7 +552,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>ChatGPT 3.5. Turbo</t>
+          <t>ChatGPT 3.5 Turbo</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -616,7 +613,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>ChatGPT 3.5. Turbo</t>
+          <t>ChatGPT 3.5 Turbo</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -803,420 +800,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>total_time_3_5</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>avg_time_3_5</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>total_time_4</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>avg_time_4</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="10.5" customWidth="1" min="1" max="1"/>
-    <col width="25.5" customWidth="1" min="2" max="2"/>
-    <col width="21" customWidth="1" min="3" max="3"/>
-    <col width="13.2" customWidth="1" min="4" max="4"/>
-    <col width="19.2" customWidth="1" min="5" max="5"/>
-    <col width="20.4" customWidth="1" min="6" max="6"/>
-    <col width="19.2" customWidth="1" min="7" max="7"/>
-    <col width="20.4" customWidth="1" min="8" max="8"/>
-    <col width="13.2" customWidth="1" min="9" max="9"/>
-    <col width="9.6" customWidth="1" min="10" max="10"/>
-    <col width="12" customWidth="1" min="11" max="11"/>
-    <col width="15" customWidth="1" min="12" max="12"/>
-    <col width="15.6" customWidth="1" min="13" max="13"/>
-    <col width="15.6" customWidth="1" min="14" max="14"/>
-    <col width="25.2" customWidth="1" min="15" max="15"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>Model</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>Redundancy Part</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>Ground Truth</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>Predicted</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>True Positives</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>False Positives</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>True Negatives</t>
-        </is>
-      </c>
-      <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>False Negatives</t>
-        </is>
-      </c>
-      <c r="I1" s="2" t="inlineStr">
-        <is>
-          <t>Precision</t>
-        </is>
-      </c>
-      <c r="J1" s="2" t="inlineStr">
-        <is>
-          <t>Recall</t>
-        </is>
-      </c>
-      <c r="K1" s="2" t="inlineStr">
-        <is>
-          <t>F1 Score</t>
-        </is>
-      </c>
-      <c r="L1" s="2" t="inlineStr">
-        <is>
-          <t>Accuracy</t>
-        </is>
-      </c>
-      <c r="M1" s="2" t="inlineStr">
-        <is>
-          <t>Sensitivity</t>
-        </is>
-      </c>
-      <c r="N1" s="2" t="inlineStr">
-        <is>
-          <t>Specificity</t>
-        </is>
-      </c>
-      <c r="O1" s="2" t="inlineStr">
-        <is>
-          <t>False Positive Rate</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>ChatGPT 3.5 Turbo</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>Main Part</t>
-        </is>
-      </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>[0]</t>
-        </is>
-      </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>[1]</t>
-        </is>
-      </c>
-      <c r="E2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" s="3" t="inlineStr">
-        <is>
-          <t>[0. 1.]</t>
-        </is>
-      </c>
-      <c r="J2" s="3" t="inlineStr">
-        <is>
-          <t>[1. 0.]</t>
-        </is>
-      </c>
-      <c r="K2" s="3" t="inlineStr">
-        <is>
-          <t>0.</t>
-        </is>
-      </c>
-      <c r="L2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>ChatGPT 3.5 Turbo</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>Benefit</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>[1]</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>[1]</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3" t="inlineStr">
-        <is>
-          <t>[1. 1.]</t>
-        </is>
-      </c>
-      <c r="J3" s="3" t="inlineStr">
-        <is>
-          <t>[1. 0.]</t>
-        </is>
-      </c>
-      <c r="K3" s="3" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="L3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="M3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="N3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>ChatGPT 4 Turbo</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>Main Part</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="inlineStr">
-        <is>
-          <t>[0]</t>
-        </is>
-      </c>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t>[1]</t>
-        </is>
-      </c>
-      <c r="E4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3" t="inlineStr">
-        <is>
-          <t>[0. 1.]</t>
-        </is>
-      </c>
-      <c r="J4" s="3" t="inlineStr">
-        <is>
-          <t>[1. 0.]</t>
-        </is>
-      </c>
-      <c r="K4" s="3" t="inlineStr">
-        <is>
-          <t>0.</t>
-        </is>
-      </c>
-      <c r="L4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" s="3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>ChatGPT 4 Turbo</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>Benefit</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="inlineStr">
-        <is>
-          <t>[0]</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
-          <t>[1]</t>
-        </is>
-      </c>
-      <c r="E5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3" t="inlineStr">
-        <is>
-          <t>[0. 1.]</t>
-        </is>
-      </c>
-      <c r="J5" s="3" t="inlineStr">
-        <is>
-          <t>[1. 0.]</t>
-        </is>
-      </c>
-      <c r="K5" s="3" t="inlineStr">
-        <is>
-          <t>0.</t>
-        </is>
-      </c>
-      <c r="L5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" s="3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:O1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1429,7 +1012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1568,7 +1151,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
improved passing function to multiprocessing
</commit_message>
<xml_diff>
--- a/src/output_detections_highlighting_without_annotations.xlsx
+++ b/src/output_detections_highlighting_without_annotations.xlsx
@@ -6,18 +6,18 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Time Consup. Anlys.S." sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Only US-Result" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Only US-False Pos. Neg." sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Only US-True Pos." sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Time Consup." sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Only US-Result" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Only US-False Pos. Neg." sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Only US-True Pos." sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Time Consup." sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Time Consup. Anlys.S." sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Time Consup. Anlys.S.'!$A$1:$H$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Only US-Result'!$A$1:$O$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Only US-False Pos. Neg.'!$A$1:$L$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Only US-True Pos.'!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Time Consup.'!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Only US-Result'!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Only US-False Pos. Neg.'!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Only US-True Pos.'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Time Consup.'!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Time Consup. Anlys.S.'!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
@@ -520,258 +520,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="13.44140625" customWidth="1" min="1" max="1"/>
-    <col width="16.44140625" customWidth="1" min="2" max="2"/>
-    <col width="22.44140625" customWidth="1" min="3" max="3"/>
-    <col width="28.44140625" customWidth="1" min="4" max="4"/>
-    <col width="19.44140625" customWidth="1" min="5" max="5"/>
-    <col width="21" customWidth="1" min="6" max="6"/>
-    <col width="13.44140625" customWidth="1" min="7" max="8"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="18" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Dataset</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Run Count</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Model Version</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Threading Enabled</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Nanoseconds</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Milliseconds</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Seconds</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Minutes</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>#G02#</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>#G03#</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>#G04#</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>#G02#</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>#G03#</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>#G04#</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:H1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1101,7 +849,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2101,7 +1849,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2304,7 +2052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2603,4 +2351,257 @@
   <autoFilter ref="A1:J1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13.5" customWidth="1" min="1" max="1"/>
+    <col width="16.5" customWidth="1" min="2" max="2"/>
+    <col width="22.5" customWidth="1" min="3" max="3"/>
+    <col width="28.5" customWidth="1" min="4" max="4"/>
+    <col width="19.5" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="6" max="6"/>
+    <col width="13.5" customWidth="1" min="7" max="7"/>
+    <col width="13.5" customWidth="1" min="8" max="8"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="8" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="B1" s="8" t="inlineStr">
+        <is>
+          <t>Run Count</t>
+        </is>
+      </c>
+      <c r="C1" s="8" t="inlineStr">
+        <is>
+          <t>Model Version</t>
+        </is>
+      </c>
+      <c r="D1" s="8" t="inlineStr">
+        <is>
+          <t>Threading Enabled</t>
+        </is>
+      </c>
+      <c r="E1" s="8" t="inlineStr">
+        <is>
+          <t>Nanoseconds</t>
+        </is>
+      </c>
+      <c r="F1" s="8" t="inlineStr">
+        <is>
+          <t>Milliseconds</t>
+        </is>
+      </c>
+      <c r="G1" s="8" t="inlineStr">
+        <is>
+          <t>Seconds</t>
+        </is>
+      </c>
+      <c r="H1" s="8" t="inlineStr">
+        <is>
+          <t>Minutes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>#G02#</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>#G03#</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>#G04#</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>#G02#</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>#G03#</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>#G04#</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Repaired Timesum and Prepaired analyse scripts
</commit_message>
<xml_diff>
--- a/src/output_detections_highlighting_without_annotations.xlsx
+++ b/src/output_detections_highlighting_without_annotations.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1900" yWindow="1900" windowWidth="28800" windowHeight="15410" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Only US-Result" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Only US-False Pos. Neg." sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Only US-True Pos." sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Time Consup." sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Time Consup. Anlys.S." sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Time Consup. Anlys.S." sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Only US-Result" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Only US-False Pos. Neg." sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Only US-True Pos." sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Time Consup." sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Only US-Result'!$A$1:$O$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Only US-False Pos. Neg.'!$A$1:$L$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Only US-True Pos.'!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Time Consup.'!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Time Consup. Anlys.S.'!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Time Consup. Anlys.S.'!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Only US-Result'!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Only US-False Pos. Neg.'!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Only US-True Pos.'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Time Consup.'!$A$1:$J$1</definedName>
   </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
@@ -26,18 +26,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="14"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -72,27 +67,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -120,39 +100,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -520,6 +497,265 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13.5" customWidth="1" min="1" max="1"/>
+    <col width="16.5" customWidth="1" min="2" max="2"/>
+    <col width="22.5" customWidth="1" min="3" max="3"/>
+    <col width="28.5" customWidth="1" min="4" max="4"/>
+    <col width="19.5" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="6" max="6"/>
+    <col width="13.5" customWidth="1" min="7" max="7"/>
+    <col width="13.5" customWidth="1" min="8" max="8"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="7" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Run Count</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>Model Version</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>Threading Enabled</t>
+        </is>
+      </c>
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>Nanoseconds</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>Milliseconds</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>Seconds</t>
+        </is>
+      </c>
+      <c r="H1" s="7" t="inlineStr">
+        <is>
+          <t>Minutes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>#G02#</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>11976467500</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>11976.4675</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>11.9764675</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>0.1996077916666667</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>#G03#</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>9202548200</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>9202.548199999999</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>9.202548200000001</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>0.1533758033333333</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>#G04#</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>8843799200</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>8843.799199999999</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>8.843799199999999</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>0.1473966533333333</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>#G02#</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>22356728000</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>22356.728</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>22.356728</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>0.3726121333333333</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>#G03#</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>21636202700</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>21636.2027</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>21.6362027</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>0.3606033783333333</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>#G04#</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>gpt-3.5-turbo</t>
+        </is>
+      </c>
+      <c r="D7" s="1" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>21587674400</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>21587.6744</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>21.5876744</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>0.3597945733333334</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -547,299 +783,299 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="8" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="B1" s="8" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>Redundancy Part</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>Ground Truth</t>
         </is>
       </c>
-      <c r="D1" s="8" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>Predicted</t>
         </is>
       </c>
-      <c r="E1" s="8" t="inlineStr">
+      <c r="E1" s="7" t="inlineStr">
         <is>
           <t>True Positives</t>
         </is>
       </c>
-      <c r="F1" s="9" t="inlineStr">
+      <c r="F1" s="8" t="inlineStr">
         <is>
           <t>False Positives</t>
         </is>
       </c>
-      <c r="G1" s="8" t="inlineStr">
+      <c r="G1" s="7" t="inlineStr">
         <is>
           <t>True Negatives</t>
         </is>
       </c>
-      <c r="H1" s="9" t="inlineStr">
+      <c r="H1" s="8" t="inlineStr">
         <is>
           <t>False Negatives</t>
         </is>
       </c>
-      <c r="I1" s="8" t="inlineStr">
+      <c r="I1" s="7" t="inlineStr">
         <is>
           <t>Precision</t>
         </is>
       </c>
-      <c r="J1" s="8" t="inlineStr">
+      <c r="J1" s="7" t="inlineStr">
         <is>
           <t>Recall</t>
         </is>
       </c>
-      <c r="K1" s="8" t="inlineStr">
+      <c r="K1" s="7" t="inlineStr">
         <is>
           <t>F1 Score</t>
         </is>
       </c>
-      <c r="L1" s="8" t="inlineStr">
+      <c r="L1" s="7" t="inlineStr">
         <is>
           <t>Accuracy</t>
         </is>
       </c>
-      <c r="M1" s="8" t="inlineStr">
+      <c r="M1" s="7" t="inlineStr">
         <is>
           <t>Sensitivity</t>
         </is>
       </c>
-      <c r="N1" s="8" t="inlineStr">
+      <c r="N1" s="7" t="inlineStr">
         <is>
           <t>Specificity</t>
         </is>
       </c>
-      <c r="O1" s="8" t="inlineStr">
+      <c r="O1" s="7" t="inlineStr">
         <is>
           <t>False Positive Rate</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>ChatGPT 3.5 Turbo</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>Main Part</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>[0 0 0 ... 0 0 0]</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>[0 0 0 ... 0 0 0]</t>
         </is>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="10" t="n">
+      <c r="F2" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="1" t="n">
         <v>4460</v>
       </c>
-      <c r="H2" s="10" t="n">
+      <c r="H2" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="I2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J2" s="2" t="n">
+      <c r="J2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K2" s="2" t="n">
+      <c r="K2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L2" s="2" t="n">
+      <c r="L2" s="1" t="n">
         <v>0.9984329527647191</v>
       </c>
-      <c r="M2" s="2" t="n">
+      <c r="M2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="N2" s="2" t="n">
+      <c r="N2" s="1" t="n">
         <v>0.9988801791713325</v>
       </c>
-      <c r="O2" s="2" t="n">
+      <c r="O2" s="1" t="n">
         <v>0.001119820828667413</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>ChatGPT 3.5 Turbo</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" s="1" t="inlineStr">
         <is>
           <t>Benefit</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" s="1" t="inlineStr">
         <is>
           <t>[0 0 0 ... 0 0 0]</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="D3" s="1" t="inlineStr">
         <is>
           <t>[0 0 0 ... 0 0 0]</t>
         </is>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F3" s="10" t="n">
+      <c r="F3" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="1" t="n">
         <v>4459</v>
       </c>
-      <c r="H3" s="10" t="n">
+      <c r="H3" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="I3" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="J3" s="2" t="n">
+      <c r="J3" s="1" t="n">
         <v>0.3333333333333333</v>
       </c>
-      <c r="K3" s="2" t="n">
+      <c r="K3" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="L3" s="2" t="n">
+      <c r="L3" s="1" t="n">
         <v>0.9986568166554735</v>
       </c>
-      <c r="M3" s="2" t="n">
+      <c r="M3" s="1" t="n">
         <v>0.3333333333333333</v>
       </c>
-      <c r="N3" s="2" t="n">
+      <c r="N3" s="1" t="n">
         <v>0.9995516700291415</v>
       </c>
-      <c r="O3" s="2" t="n">
+      <c r="O3" s="1" t="n">
         <v>0.0004483299708585519</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>ChatGPT 4</t>
         </is>
       </c>
-      <c r="B4" s="2" t="inlineStr">
+      <c r="B4" s="1" t="inlineStr">
         <is>
           <t>Main Part</t>
         </is>
       </c>
-      <c r="C4" s="2" t="inlineStr">
+      <c r="C4" s="1" t="inlineStr">
         <is>
           <t>[0]</t>
         </is>
       </c>
-      <c r="D4" s="2" t="inlineStr">
+      <c r="D4" s="1" t="inlineStr">
         <is>
           <t>[1]</t>
         </is>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="10" t="n">
+      <c r="F4" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="10" t="n">
+      <c r="H4" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="I4" s="2" t="n">
+      <c r="I4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J4" s="2" t="n">
+      <c r="J4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K4" s="2" t="n">
+      <c r="K4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L4" s="2" t="n">
+      <c r="L4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M4" s="2" t="n">
+      <c r="M4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="N4" s="2" t="n">
+      <c r="N4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="O4" s="2" t="n">
+      <c r="O4" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>ChatGPT 4o</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B5" s="1" t="inlineStr">
         <is>
           <t>Benefit</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C5" s="1" t="inlineStr">
         <is>
           <t>[0]</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr">
+      <c r="D5" s="1" t="inlineStr">
         <is>
           <t>[1]</t>
         </is>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="10" t="n">
+      <c r="F5" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H5" s="10" t="n">
+      <c r="H5" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="I5" s="2" t="n">
+      <c r="I5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J5" s="2" t="n">
+      <c r="J5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K5" s="2" t="n">
+      <c r="K5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L5" s="2" t="n">
+      <c r="L5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M5" s="2" t="n">
+      <c r="M5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="N5" s="2" t="n">
+      <c r="N5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="O5" s="2" t="n">
+      <c r="O5" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -849,7 +1085,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -879,965 +1115,965 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="11" t="inlineStr">
+      <c r="A1" s="10" t="inlineStr">
         <is>
           <t>Execution Run</t>
         </is>
       </c>
-      <c r="B1" s="11" t="inlineStr">
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="C1" s="11" t="inlineStr">
+      <c r="C1" s="10" t="inlineStr">
         <is>
           <t>Dataset</t>
         </is>
       </c>
-      <c r="D1" s="11" t="inlineStr">
+      <c r="D1" s="10" t="inlineStr">
         <is>
           <t>False Type</t>
         </is>
       </c>
-      <c r="E1" s="11" t="inlineStr">
+      <c r="E1" s="10" t="inlineStr">
         <is>
           <t>Main Part or Benefit</t>
         </is>
       </c>
-      <c r="F1" s="11" t="inlineStr">
+      <c r="F1" s="10" t="inlineStr">
         <is>
           <t>User Story Id 1</t>
         </is>
       </c>
-      <c r="G1" s="11" t="inlineStr">
+      <c r="G1" s="10" t="inlineStr">
         <is>
           <t>User Story Id 2</t>
         </is>
       </c>
-      <c r="H1" s="11" t="inlineStr">
+      <c r="H1" s="10" t="inlineStr">
         <is>
           <t>Reason from ChatGPT</t>
         </is>
       </c>
-      <c r="I1" s="11" t="inlineStr">
+      <c r="I1" s="10" t="inlineStr">
         <is>
           <t>Refered Text 1 by ChatGPT</t>
         </is>
       </c>
-      <c r="J1" s="11" t="inlineStr">
+      <c r="J1" s="10" t="inlineStr">
         <is>
           <t>Refered Text 1 from formal Approach or Original Text in case of false positive</t>
         </is>
       </c>
-      <c r="K1" s="11" t="inlineStr">
+      <c r="K1" s="10" t="inlineStr">
         <is>
           <t>Refered Text 2 by ChatGPT</t>
         </is>
       </c>
-      <c r="L1" s="11" t="inlineStr">
+      <c r="L1" s="10" t="inlineStr">
         <is>
           <t>Refered Text 2 from formal Approach or Original Text in case of false positive</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>00</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>gpt-3.5-turbo</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>G03</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>False Positive</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
         <is>
           <t>Main Part</t>
         </is>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="1" t="n">
         <v>326</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="1" t="n">
         <v>353</v>
       </c>
-      <c r="H2" s="2" t="inlineStr">
+      <c r="H2" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) The redundancy arises from the repetition of the concept of reviewing for compliance expressed in slightly different ways for emphasis or to cater to different audiences.
 </t>
         </is>
       </c>
-      <c r="I2" s="2" t="inlineStr">
+      <c r="I2" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) As a Staff member, I want to Assign an Application for Detailed Review
 </t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
+      <c r="J2" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as a staff member, i want to assign an application for detailed review, so that i can #review# them for #compliance# and subsequently approved or denied.</t>
         </is>
       </c>
-      <c r="K2" s="2" t="inlineStr">
+      <c r="K2" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) As a Plan Review Staff member, I want to Review Plans
 </t>
         </is>
       </c>
-      <c r="L2" s="2" t="inlineStr">
+      <c r="L2" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as a plan review staff member, i want to review plans, so that i can #review# them for #compliance# and either approve, or fail or deny the plans and record any conditions, clearances, or corrections needed from the applicant.</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>00</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" s="1" t="inlineStr">
         <is>
           <t>gpt-3.5-turbo</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" s="1" t="inlineStr">
         <is>
           <t>G03</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="D3" s="1" t="inlineStr">
         <is>
           <t>False Negative</t>
         </is>
       </c>
-      <c r="E3" s="2" t="inlineStr">
+      <c r="E3" s="1" t="inlineStr">
         <is>
           <t>Benefit</t>
         </is>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="1" t="n">
         <v>331</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="1" t="n">
         <v>344</v>
       </c>
-      <c r="H3" s="2" t="inlineStr">
+      <c r="H3" s="1" t="inlineStr">
         <is>
           <t>LLM did not return an answere as it did not detect a redundancy</t>
         </is>
       </c>
-      <c r="I3" s="2" t="inlineStr">
+      <c r="I3" s="1" t="inlineStr">
         <is>
           <t>LLM did not return an answere as it did not detect a redundancy</t>
         </is>
       </c>
-      <c r="J3" s="2" t="inlineStr">
+      <c r="J3" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as a staff member, i want to manage approved proffers, so that i can #ensure# #compliance# with and satisfaction of the proffer in the future.</t>
         </is>
       </c>
-      <c r="K3" s="2" t="inlineStr">
+      <c r="K3" s="1" t="inlineStr">
         <is>
           <t>LLM did not return an answere as it did not detect a redundancy</t>
         </is>
       </c>
-      <c r="L3" s="2" t="inlineStr">
+      <c r="L3" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as a staff member, i want to manage affidavits, so that i can #ensure# #compliance# with the requirements prior to the hearing.</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>00</t>
         </is>
       </c>
-      <c r="B4" s="2" t="inlineStr">
+      <c r="B4" s="1" t="inlineStr">
         <is>
           <t>gpt-3.5-turbo</t>
         </is>
       </c>
-      <c r="C4" s="2" t="inlineStr">
+      <c r="C4" s="1" t="inlineStr">
         <is>
           <t>G03</t>
         </is>
       </c>
-      <c r="D4" s="2" t="inlineStr">
+      <c r="D4" s="1" t="inlineStr">
         <is>
           <t>False Positive</t>
         </is>
       </c>
-      <c r="E4" s="2" t="inlineStr">
+      <c r="E4" s="1" t="inlineStr">
         <is>
           <t>Benefit</t>
         </is>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="1" t="n">
         <v>345</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="1" t="n">
         <v>346</v>
       </c>
-      <c r="H4" s="2" t="inlineStr">
+      <c r="H4" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) The redundancy in benefits lies in the repetition of ensuring that all pre-hearing requirements are satisfied, which is redundant as it is already mentioned in both stories.
 </t>
         </is>
       </c>
-      <c r="I4" s="2" t="inlineStr">
+      <c r="I4" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) I can ensure all pre-hearing requirements are satisfied in time for the hearing.
 </t>
         </is>
       </c>
-      <c r="J4" s="2" t="inlineStr">
+      <c r="J4" s="1" t="inlineStr">
         <is>
           <t>As a Staff member, I want to Prepare for and Support Hearing Execution, so that I can ensure all pre-hearing requirements are satisfied and staff and Applicant are ready for the hearing.</t>
         </is>
       </c>
-      <c r="K4" s="2" t="inlineStr">
+      <c r="K4" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) I can ensure all pre-hearing requirements are satisfied and staff and Applicant are ready for the hearing.
 </t>
         </is>
       </c>
-      <c r="L4" s="2" t="inlineStr">
+      <c r="L4" s="1" t="inlineStr">
         <is>
           <t>As a Staff member, I want to Prepare for and Support Hearing Execution, so that I can ensure all pre-hearing requirements are satisfied and staff and Applicant are ready for the hearing.</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>00</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B5" s="1" t="inlineStr">
         <is>
           <t>gpt-3.5-turbo</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C5" s="1" t="inlineStr">
         <is>
           <t>G04</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr">
+      <c r="D5" s="1" t="inlineStr">
         <is>
           <t>False Negative</t>
         </is>
       </c>
-      <c r="E5" s="2" t="inlineStr">
+      <c r="E5" s="1" t="inlineStr">
         <is>
           <t>Benefit</t>
         </is>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="1" t="n">
         <v>168</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="1" t="n">
         <v>175</v>
       </c>
-      <c r="H5" s="2" t="inlineStr">
+      <c r="H5" s="1" t="inlineStr">
         <is>
           <t>LLM did not return an answere as it did not detect a redundancy</t>
         </is>
       </c>
-      <c r="I5" s="2" t="inlineStr">
+      <c r="I5" s="1" t="inlineStr">
         <is>
           <t>LLM did not return an answere as it did not detect a redundancy</t>
         </is>
       </c>
-      <c r="J5" s="2" t="inlineStr">
+      <c r="J5" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as a user, i want to have a flexible pick up time, so that i can more #conveniently use# the #website#.</t>
         </is>
       </c>
-      <c r="K5" s="2" t="inlineStr">
+      <c r="K5" s="1" t="inlineStr">
         <is>
           <t>LLM did not return an answere as it did not detect a redundancy</t>
         </is>
       </c>
-      <c r="L5" s="2" t="inlineStr">
+      <c r="L5" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as a user, i want to choose a flexible pick up time, so that i can more #conveniently use# the #website#.</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>00</t>
         </is>
       </c>
-      <c r="B6" s="2" t="inlineStr">
+      <c r="B6" s="1" t="inlineStr">
         <is>
           <t>gpt-3.5-turbo</t>
         </is>
       </c>
-      <c r="C6" s="2" t="inlineStr">
+      <c r="C6" s="1" t="inlineStr">
         <is>
           <t>G04</t>
         </is>
       </c>
-      <c r="D6" s="2" t="inlineStr">
+      <c r="D6" s="1" t="inlineStr">
         <is>
           <t>False Positive</t>
         </is>
       </c>
-      <c r="E6" s="2" t="inlineStr">
+      <c r="E6" s="1" t="inlineStr">
         <is>
           <t>Main Part</t>
         </is>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="1" t="n">
         <v>168</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="G6" s="1" t="n">
         <v>175</v>
       </c>
-      <c r="H6" s="2" t="inlineStr">
+      <c r="H6" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) The redundancy arises from the repetition of the concept of choosing a flexible pick up time expressed in slightly different ways, likely for emphasis or to cater to different audiences.
 </t>
         </is>
       </c>
-      <c r="I6" s="2" t="inlineStr">
+      <c r="I6" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) As a user, I want to have a flexible pick up time
 </t>
         </is>
       </c>
-      <c r="J6" s="2" t="inlineStr">
+      <c r="J6" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as a user, i want to have a flexible pick up time, so that i can more #conveniently use# the #website#.</t>
         </is>
       </c>
-      <c r="K6" s="2" t="inlineStr">
+      <c r="K6" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) As a user, I want to choose a flexible pick up time
 </t>
         </is>
       </c>
-      <c r="L6" s="2" t="inlineStr">
+      <c r="L6" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as a user, i want to choose a flexible pick up time, so that i can more #conveniently use# the #website#.</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="inlineStr">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>00</t>
         </is>
       </c>
-      <c r="B7" s="2" t="inlineStr">
+      <c r="B7" s="1" t="inlineStr">
         <is>
           <t>gpt-3.5-turbo</t>
         </is>
       </c>
-      <c r="C7" s="2" t="inlineStr">
+      <c r="C7" s="1" t="inlineStr">
         <is>
           <t>G04</t>
         </is>
       </c>
-      <c r="D7" s="2" t="inlineStr">
+      <c r="D7" s="1" t="inlineStr">
         <is>
           <t>False Negative</t>
         </is>
       </c>
-      <c r="E7" s="2" t="inlineStr">
+      <c r="E7" s="1" t="inlineStr">
         <is>
           <t>Main Part</t>
         </is>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="1" t="n">
         <v>172</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G7" s="1" t="n">
         <v>173</v>
       </c>
-      <c r="H7" s="2" t="inlineStr">
+      <c r="H7" s="1" t="inlineStr">
         <is>
           <t>LLM did not return an answere as it did not detect a redundancy</t>
         </is>
       </c>
-      <c r="I7" s="2" t="inlineStr">
+      <c r="I7" s="1" t="inlineStr">
         <is>
           <t>LLM did not return an answere as it did not detect a redundancy</t>
         </is>
       </c>
-      <c r="J7" s="2" t="inlineStr">
+      <c r="J7" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as a #user#, i want to be able to #view# a #map display# of the public recycling bins around my #area#.</t>
         </is>
       </c>
-      <c r="K7" s="2" t="inlineStr">
+      <c r="K7" s="1" t="inlineStr">
         <is>
           <t>LLM did not return an answere as it did not detect a redundancy</t>
         </is>
       </c>
-      <c r="L7" s="2" t="inlineStr">
+      <c r="L7" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as a #user#, i want to be able to #view# a #map display# of the special waste drop off sites around my #area#.</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="inlineStr">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>00</t>
         </is>
       </c>
-      <c r="B8" s="2" t="inlineStr">
+      <c r="B8" s="1" t="inlineStr">
         <is>
           <t>gpt-3.5-turbo</t>
         </is>
       </c>
-      <c r="C8" s="2" t="inlineStr">
+      <c r="C8" s="1" t="inlineStr">
         <is>
           <t>G04</t>
         </is>
       </c>
-      <c r="D8" s="2" t="inlineStr">
+      <c r="D8" s="1" t="inlineStr">
         <is>
           <t>False Positive</t>
         </is>
       </c>
-      <c r="E8" s="2" t="inlineStr">
+      <c r="E8" s="1" t="inlineStr">
         <is>
           <t>Benefit</t>
         </is>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="1" t="n">
         <v>179</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="1" t="n">
         <v>206</v>
       </c>
-      <c r="H8" s="2" t="inlineStr">
+      <c r="H8" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) The redundancy in benefits arises from the repetition of the outcome 'users get the most recent information' and 'provide the latest information about the recycling center', which convey the same idea using slightly different wording.
 </t>
         </is>
       </c>
-      <c r="I8" s="2" t="inlineStr">
+      <c r="I8" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) As an admin, I want to be able to add or remove recycling facilities' information, so that users get the most recent information.
 </t>
         </is>
       </c>
-      <c r="J8" s="2" t="inlineStr">
+      <c r="J8" s="1" t="inlineStr">
         <is>
           <t>As a superuser, I want to update the recycling center information, so that I can provide the latest information about the recycling center.</t>
         </is>
       </c>
-      <c r="K8" s="2" t="inlineStr">
+      <c r="K8" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) As a superuser, I want to update the recycling center information, so that I can provide the latest information about the recycling center.
 </t>
         </is>
       </c>
-      <c r="L8" s="2" t="inlineStr">
+      <c r="L8" s="1" t="inlineStr">
         <is>
           <t>As a superuser, I want to update the recycling center information, so that I can provide the latest information about the recycling center.</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="inlineStr">
+      <c r="A9" s="1" t="inlineStr">
         <is>
           <t>00</t>
         </is>
       </c>
-      <c r="B9" s="2" t="inlineStr">
+      <c r="B9" s="1" t="inlineStr">
         <is>
           <t>gpt-3.5-turbo</t>
         </is>
       </c>
-      <c r="C9" s="2" t="inlineStr">
+      <c r="C9" s="1" t="inlineStr">
         <is>
           <t>G04</t>
         </is>
       </c>
-      <c r="D9" s="2" t="inlineStr">
+      <c r="D9" s="1" t="inlineStr">
         <is>
           <t>False Negative</t>
         </is>
       </c>
-      <c r="E9" s="2" t="inlineStr">
+      <c r="E9" s="1" t="inlineStr">
         <is>
           <t>Benefit</t>
         </is>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="1" t="n">
         <v>185</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="G9" s="1" t="n">
         <v>187</v>
       </c>
-      <c r="H9" s="2" t="inlineStr">
+      <c r="H9" s="1" t="inlineStr">
         <is>
           <t>LLM did not return an answere as it did not detect a redundancy</t>
         </is>
       </c>
-      <c r="I9" s="2" t="inlineStr">
+      <c r="I9" s="1" t="inlineStr">
         <is>
           <t>LLM did not return an answere as it did not detect a redundancy</t>
         </is>
       </c>
-      <c r="J9" s="2" t="inlineStr">
+      <c r="J9" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as an admin, i want to view a dashboard that monitors all the sites' statuses, so that i can #have# a #sense# of what people are doing on our sites and know the service status.</t>
         </is>
       </c>
-      <c r="K9" s="2" t="inlineStr">
+      <c r="K9" s="1" t="inlineStr">
         <is>
           <t>LLM did not return an answere as it did not detect a redundancy</t>
         </is>
       </c>
-      <c r="L9" s="2" t="inlineStr">
+      <c r="L9" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as an executive, i want to have full access to data related to my company, so that i can #have# a #sense# of my company's performance.</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="inlineStr">
+      <c r="A10" s="1" t="inlineStr">
         <is>
           <t>00</t>
         </is>
       </c>
-      <c r="B10" s="2" t="inlineStr">
+      <c r="B10" s="1" t="inlineStr">
         <is>
           <t>gpt-3.5-turbo</t>
         </is>
       </c>
-      <c r="C10" s="2" t="inlineStr">
+      <c r="C10" s="1" t="inlineStr">
         <is>
           <t>G04</t>
         </is>
       </c>
-      <c r="D10" s="2" t="inlineStr">
+      <c r="D10" s="1" t="inlineStr">
         <is>
           <t>False Negative</t>
         </is>
       </c>
-      <c r="E10" s="2" t="inlineStr">
+      <c r="E10" s="1" t="inlineStr">
         <is>
           <t>Main Part</t>
         </is>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="1" t="n">
         <v>189</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="G10" s="1" t="n">
         <v>213</v>
       </c>
-      <c r="H10" s="2" t="inlineStr">
+      <c r="H10" s="1" t="inlineStr">
         <is>
           <t>LLM did not return an answere as it did not detect a redundancy</t>
         </is>
       </c>
-      <c r="I10" s="2" t="inlineStr">
+      <c r="I10" s="1" t="inlineStr">
         <is>
           <t>LLM did not return an answere as it did not detect a redundancy</t>
         </is>
       </c>
-      <c r="J10" s="2" t="inlineStr">
+      <c r="J10" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as an employee from the hr department, i want to #have# #access# to the full information of all employees working for this business.</t>
         </is>
       </c>
-      <c r="K10" s="2" t="inlineStr">
+      <c r="K10" s="1" t="inlineStr">
         <is>
           <t>LLM did not return an answere as it did not detect a redundancy</t>
         </is>
       </c>
-      <c r="L10" s="2" t="inlineStr">
+      <c r="L10" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as a recyclingfacility representative, i want to #have# #access# to user stats and schedules, so that i can adjust my hours and/or upgrade equipment and capacity in order to be able to accomodate larger amounts of recyclable materials.</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="inlineStr">
+      <c r="A11" s="1" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
-      <c r="B11" s="2" t="inlineStr">
+      <c r="B11" s="1" t="inlineStr">
         <is>
           <t>gpt-3.5-turbo</t>
         </is>
       </c>
-      <c r="C11" s="2" t="inlineStr">
+      <c r="C11" s="1" t="inlineStr">
         <is>
           <t>G03</t>
         </is>
       </c>
-      <c r="D11" s="2" t="inlineStr">
+      <c r="D11" s="1" t="inlineStr">
         <is>
           <t>False Positive</t>
         </is>
       </c>
-      <c r="E11" s="2" t="inlineStr">
+      <c r="E11" s="1" t="inlineStr">
         <is>
           <t>Main Part</t>
         </is>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="1" t="n">
         <v>326</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G11" s="1" t="n">
         <v>353</v>
       </c>
-      <c r="H11" s="2" t="inlineStr">
+      <c r="H11" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) The redundancy arises from the repetition of the action of reviewing for compliance and making a decision, expressed in slightly different ways for emphasis or to cater to different audiences.
 </t>
         </is>
       </c>
-      <c r="I11" s="2" t="inlineStr">
+      <c r="I11" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) As a Staff member, I want to Assign an Application for Detailed Review
 </t>
         </is>
       </c>
-      <c r="J11" s="2" t="inlineStr">
+      <c r="J11" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as a staff member, i want to assign an application for detailed review, so that i can #review# them for #compliance# and subsequently approved or denied.</t>
         </is>
       </c>
-      <c r="K11" s="2" t="inlineStr">
+      <c r="K11" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) As a Plan Review Staff member, I want to Review Plans
 </t>
         </is>
       </c>
-      <c r="L11" s="2" t="inlineStr">
+      <c r="L11" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as a plan review staff member, i want to review plans, so that i can #review# them for #compliance# and either approve, or fail or deny the plans and record any conditions, clearances, or corrections needed from the applicant.</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="inlineStr">
+      <c r="A12" s="1" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
-      <c r="B12" s="2" t="inlineStr">
+      <c r="B12" s="1" t="inlineStr">
         <is>
           <t>gpt-3.5-turbo</t>
         </is>
       </c>
-      <c r="C12" s="2" t="inlineStr">
+      <c r="C12" s="1" t="inlineStr">
         <is>
           <t>G03</t>
         </is>
       </c>
-      <c r="D12" s="2" t="inlineStr">
+      <c r="D12" s="1" t="inlineStr">
         <is>
           <t>False Negative</t>
         </is>
       </c>
-      <c r="E12" s="2" t="inlineStr">
+      <c r="E12" s="1" t="inlineStr">
         <is>
           <t>Benefit</t>
         </is>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="1" t="n">
         <v>331</v>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="G12" s="1" t="n">
         <v>344</v>
       </c>
-      <c r="H12" s="2" t="inlineStr">
+      <c r="H12" s="1" t="inlineStr">
         <is>
           <t>LLM did not return an answere as it did not detect a redundancy</t>
         </is>
       </c>
-      <c r="I12" s="2" t="inlineStr">
+      <c r="I12" s="1" t="inlineStr">
         <is>
           <t>LLM did not return an answere as it did not detect a redundancy</t>
         </is>
       </c>
-      <c r="J12" s="2" t="inlineStr">
+      <c r="J12" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as a staff member, i want to manage approved proffers, so that i can #ensure# #compliance# with and satisfaction of the proffer in the future.</t>
         </is>
       </c>
-      <c r="K12" s="2" t="inlineStr">
+      <c r="K12" s="1" t="inlineStr">
         <is>
           <t>LLM did not return an answere as it did not detect a redundancy</t>
         </is>
       </c>
-      <c r="L12" s="2" t="inlineStr">
+      <c r="L12" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as a staff member, i want to manage affidavits, so that i can #ensure# #compliance# with the requirements prior to the hearing.</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="inlineStr">
+      <c r="A13" s="1" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
-      <c r="B13" s="2" t="inlineStr">
+      <c r="B13" s="1" t="inlineStr">
         <is>
           <t>gpt-3.5-turbo</t>
         </is>
       </c>
-      <c r="C13" s="2" t="inlineStr">
+      <c r="C13" s="1" t="inlineStr">
         <is>
           <t>G03</t>
         </is>
       </c>
-      <c r="D13" s="2" t="inlineStr">
+      <c r="D13" s="1" t="inlineStr">
         <is>
           <t>False Positive</t>
         </is>
       </c>
-      <c r="E13" s="2" t="inlineStr">
+      <c r="E13" s="1" t="inlineStr">
         <is>
           <t>Main Part</t>
         </is>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="F13" s="1" t="n">
         <v>352</v>
       </c>
-      <c r="G13" s="2" t="n">
+      <c r="G13" s="1" t="n">
         <v>353</v>
       </c>
-      <c r="H13" s="2" t="inlineStr">
+      <c r="H13" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) The redundancy arises from the repetition of the concept of reviewing plans, expressed in slightly different ways for emphasis or to cater to different audiences.
 </t>
         </is>
       </c>
-      <c r="I13" s="2" t="inlineStr">
+      <c r="I13" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) As a Plan Review Staff member, I want to successfully Conduct a Plan Review Meeting with the Applicant and record the outcome
 </t>
         </is>
       </c>
-      <c r="J13" s="2" t="inlineStr">
+      <c r="J13" s="1" t="inlineStr">
         <is>
           <t>As a Plan Review Staff member, I want to Review Plans, so that I can review them for compliance and either approve, or fail or deny the plans and record any conditions, clearances, or corrections needed from the Applicant.</t>
         </is>
       </c>
-      <c r="K13" s="2" t="inlineStr">
+      <c r="K13" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) As a Plan Review Staff member, I want to Review Plans
 </t>
         </is>
       </c>
-      <c r="L13" s="2" t="inlineStr">
+      <c r="L13" s="1" t="inlineStr">
         <is>
           <t>As a Plan Review Staff member, I want to Review Plans, so that I can review them for compliance and either approve, or fail or deny the plans and record any conditions, clearances, or corrections needed from the Applicant.</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="inlineStr">
+      <c r="A14" s="1" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
-      <c r="B14" s="2" t="inlineStr">
+      <c r="B14" s="1" t="inlineStr">
         <is>
           <t>gpt-3.5-turbo</t>
         </is>
       </c>
-      <c r="C14" s="2" t="inlineStr">
+      <c r="C14" s="1" t="inlineStr">
         <is>
           <t>G03</t>
         </is>
       </c>
-      <c r="D14" s="2" t="inlineStr">
+      <c r="D14" s="1" t="inlineStr">
         <is>
           <t>False Positive</t>
         </is>
       </c>
-      <c r="E14" s="2" t="inlineStr">
+      <c r="E14" s="1" t="inlineStr">
         <is>
           <t>Main Part</t>
         </is>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="1" t="n">
         <v>353</v>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="G14" s="1" t="n">
         <v>356</v>
       </c>
-      <c r="H14" s="2" t="inlineStr">
+      <c r="H14" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) The redundancy arises from the repetition of the role 'Plan Review Staff member' and the action 'Review' in both User Stories, with slight variations in the context.
 </t>
         </is>
       </c>
-      <c r="I14" s="2" t="inlineStr">
+      <c r="I14" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) As a Plan Review Staff member, I want to Review Plans
 </t>
         </is>
       </c>
-      <c r="J14" s="2" t="inlineStr">
+      <c r="J14" s="1" t="inlineStr">
         <is>
           <t>As a Plan Review Staff member, I want to Track the Completion of Required Plan Reviews, so that I can ensure all plan review tasks are completed, results have been sent to the Applicant and any downstream steps are initiated such has a final review or payment for permit issuance.</t>
         </is>
       </c>
-      <c r="K14" s="2" t="inlineStr">
+      <c r="K14" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) As a Plan Review Staff member, I want to Track the Completion of Required Plan Reviews
 </t>
         </is>
       </c>
-      <c r="L14" s="2" t="inlineStr">
+      <c r="L14" s="1" t="inlineStr">
         <is>
           <t>As a Plan Review Staff member, I want to Track the Completion of Required Plan Reviews, so that I can ensure all plan review tasks are completed, results have been sent to the Applicant and any downstream steps are initiated such has a final review or payment for permit issuance.</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="inlineStr">
+      <c r="A15" s="1" t="inlineStr">
         <is>
           <t>00</t>
         </is>
       </c>
-      <c r="B15" s="2" t="inlineStr">
+      <c r="B15" s="1" t="inlineStr">
         <is>
           <t>gpt-4-turbo</t>
         </is>
       </c>
-      <c r="C15" s="2" t="inlineStr">
+      <c r="C15" s="1" t="inlineStr">
         <is>
           <t>G11</t>
         </is>
       </c>
-      <c r="D15" s="2" t="inlineStr">
+      <c r="D15" s="1" t="inlineStr">
         <is>
           <t>False Positive</t>
         </is>
       </c>
-      <c r="E15" s="2" t="inlineStr">
+      <c r="E15" s="1" t="inlineStr">
         <is>
           <t>Main Part</t>
         </is>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F15" s="1" t="n">
         <v>590</v>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="G15" s="1" t="n">
         <v>591</v>
       </c>
-      <c r="H15" s="2" t="inlineStr">
+      <c r="H15" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) Dummy Value Describtion
 1.) The redundancy here stems from the repetition of the testing action and the tested entity, expressed in slightly different ways, likely for emphasis or to accommodate different perspectives
 </t>
         </is>
       </c>
-      <c r="I15" s="2" t="inlineStr">
+      <c r="I15" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) As a User, I want to verify myself
 1.) As a software tester, I want to begin user testing
 </t>
         </is>
       </c>
-      <c r="J15" s="2" t="inlineStr">
+      <c r="J15" s="1" t="inlineStr">
         <is>
           <t>As a developer, I want to have the subdomain beta.nsf.gov be set up, so that I can deploy a beta site to it.</t>
         </is>
       </c>
-      <c r="K15" s="2" t="inlineStr">
+      <c r="K15" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) As an application User, I want to verify that I am who I am
 1.) As a tester, I want to begin testing the software
 </t>
         </is>
       </c>
-      <c r="L15" s="2" t="inlineStr">
+      <c r="L15" s="1" t="inlineStr">
         <is>
           <t>As a developer, I want to have the subdomain beta.nsf.gov be set up, so that I can deploy a beta site to it.</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="inlineStr">
+      <c r="A16" s="1" t="inlineStr">
         <is>
           <t>00</t>
         </is>
       </c>
-      <c r="B16" s="2" t="inlineStr">
+      <c r="B16" s="1" t="inlineStr">
         <is>
           <t>gpt-4-turbo</t>
         </is>
       </c>
-      <c r="C16" s="2" t="inlineStr">
+      <c r="C16" s="1" t="inlineStr">
         <is>
           <t>G11</t>
         </is>
       </c>
-      <c r="D16" s="2" t="inlineStr">
+      <c r="D16" s="1" t="inlineStr">
         <is>
           <t>False Positive</t>
         </is>
       </c>
-      <c r="E16" s="2" t="inlineStr">
+      <c r="E16" s="1" t="inlineStr">
         <is>
           <t>Benefit</t>
         </is>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="F16" s="1" t="n">
         <v>590</v>
       </c>
-      <c r="G16" s="2" t="n">
+      <c r="G16" s="1" t="n">
         <v>591</v>
       </c>
-      <c r="H16" s="2" t="inlineStr">
+      <c r="H16" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) The redundancy in these sentences lies in the repetition of the action ('login') and the destination ('webpage' and 'website'), which convey the same idea using slightly different wording.
 1.) Dummy Value Describtion
 </t>
         </is>
       </c>
-      <c r="I16" s="2" t="inlineStr">
+      <c r="I16" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) I can login into the webpage.
 1.) I can print a document
 </t>
         </is>
       </c>
-      <c r="J16" s="2" t="inlineStr">
+      <c r="J16" s="1" t="inlineStr">
         <is>
           <t>As a developer, I want to have the subdomain beta.nsf.gov be set up, so that I can deploy a beta site to it.</t>
         </is>
       </c>
-      <c r="K16" s="2" t="inlineStr">
+      <c r="K16" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) I could login into the website
 1.) I can give the order to print
 </t>
         </is>
       </c>
-      <c r="L16" s="2" t="inlineStr">
+      <c r="L16" s="1" t="inlineStr">
         <is>
           <t>As a developer, I want to have the subdomain beta.nsf.gov be set up, so that I can deploy a beta site to it.</t>
         </is>
@@ -1849,7 +2085,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1878,169 +2114,169 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="8" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Execution Run</t>
         </is>
       </c>
-      <c r="B1" s="8" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>Dataset</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="D1" s="8" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>Main Part or Benefit</t>
         </is>
       </c>
-      <c r="E1" s="8" t="inlineStr">
+      <c r="E1" s="7" t="inlineStr">
         <is>
           <t>User Story Id 1</t>
         </is>
       </c>
-      <c r="F1" s="8" t="inlineStr">
+      <c r="F1" s="7" t="inlineStr">
         <is>
           <t>User Story Id 2</t>
         </is>
       </c>
-      <c r="G1" s="8" t="inlineStr">
+      <c r="G1" s="7" t="inlineStr">
         <is>
           <t>Reason from ChatGPT</t>
         </is>
       </c>
-      <c r="H1" s="8" t="inlineStr">
+      <c r="H1" s="7" t="inlineStr">
         <is>
           <t>Refered Text 1 by ChatGPT</t>
         </is>
       </c>
-      <c r="I1" s="8" t="inlineStr">
+      <c r="I1" s="7" t="inlineStr">
         <is>
           <t>Refered Text 1 from formal Approach</t>
         </is>
       </c>
-      <c r="J1" s="8" t="inlineStr">
+      <c r="J1" s="7" t="inlineStr">
         <is>
           <t>Refered Text 2 by ChatGPT</t>
         </is>
       </c>
-      <c r="K1" s="8" t="inlineStr">
+      <c r="K1" s="7" t="inlineStr">
         <is>
           <t>Refered Text 2 from formal Approach</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>00</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>G03</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>gpt-3.5-turbo</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>Benefit</t>
         </is>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="1" t="n">
         <v>326</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="1" t="n">
         <v>353</v>
       </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="G2" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) The redundancy in these sentences lies in the repetition of the outcome ('review for compliance') and the actions ('approve' and 'deny'), which convey the same idea using slightly different wording.
 </t>
         </is>
       </c>
-      <c r="H2" s="2" t="inlineStr">
+      <c r="H2" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) so that I can review the for compliance and subsequently approved or denied
 </t>
         </is>
       </c>
-      <c r="I2" s="2" t="inlineStr">
+      <c r="I2" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as a staff member, i want to assign an application for detailed review, so that i can #review# them for #compliance# and subsequently approved or denied.</t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
+      <c r="J2" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) so that I can review them for compliance and either approve, or fail or deny the plans and record any conditions, clearances, or corrections needed from the Applicant
 </t>
         </is>
       </c>
-      <c r="K2" s="2" t="inlineStr">
+      <c r="K2" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as a plan review staff member, i want to review plans, so that i can #review# them for #compliance# and either approve, or fail or deny the plans and record any conditions, clearances, or corrections needed from the applicant.</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" s="1" t="inlineStr">
         <is>
           <t>G03</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" s="1" t="inlineStr">
         <is>
           <t>gpt-3.5-turbo</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="D3" s="1" t="inlineStr">
         <is>
           <t>Benefit</t>
         </is>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="1" t="n">
         <v>326</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="1" t="n">
         <v>353</v>
       </c>
-      <c r="G3" s="2" t="inlineStr">
+      <c r="G3" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) The redundancy in these sentences lies in the repetition of the outcome ('review for compliance') and the decision-making process ('approve or deny'), which convey the same idea using slightly different wording.
 </t>
         </is>
       </c>
-      <c r="H3" s="2" t="inlineStr">
+      <c r="H3" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) so that I can review the for compliance and subsequently approved or denied
 </t>
         </is>
       </c>
-      <c r="I3" s="2" t="inlineStr">
+      <c r="I3" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as a staff member, i want to assign an application for detailed review, so that i can #review# them for #compliance# and subsequently approved or denied.</t>
         </is>
       </c>
-      <c r="J3" s="2" t="inlineStr">
+      <c r="J3" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) so that I can review them for compliance and either approve, or fail or deny the plans and record any conditions, clearances, or corrections needed from the Applicant
 </t>
         </is>
       </c>
-      <c r="K3" s="2" t="inlineStr">
+      <c r="K3" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> as a plan review staff member, i want to review plans, so that i can #review# them for #compliance# and either approve, or fail or deny the plans and record any conditions, clearances, or corrections needed from the applicant.</t>
         </is>
@@ -2052,7 +2288,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2080,270 +2316,270 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="8" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Version</t>
         </is>
       </c>
-      <c r="B1" s="8" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>Groups</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>Total Time (ns)</t>
         </is>
       </c>
-      <c r="D1" s="8" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>Avg Time (ns)</t>
         </is>
       </c>
-      <c r="E1" s="8" t="inlineStr">
+      <c r="E1" s="7" t="inlineStr">
         <is>
           <t>Total Time (ms)</t>
         </is>
       </c>
-      <c r="F1" s="8" t="inlineStr">
+      <c r="F1" s="7" t="inlineStr">
         <is>
           <t>Avg Time (ms)</t>
         </is>
       </c>
-      <c r="G1" s="8" t="inlineStr">
+      <c r="G1" s="7" t="inlineStr">
         <is>
           <t>Total Time (s)</t>
         </is>
       </c>
-      <c r="H1" s="8" t="inlineStr">
+      <c r="H1" s="7" t="inlineStr">
         <is>
           <t>Avg Time (s)</t>
         </is>
       </c>
-      <c r="I1" s="8" t="inlineStr">
+      <c r="I1" s="7" t="inlineStr">
         <is>
           <t>Total Time (m)</t>
         </is>
       </c>
-      <c r="J1" s="8" t="inlineStr">
+      <c r="J1" s="7" t="inlineStr">
         <is>
           <t>Avg Time (m)</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>v3.5</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>All sets</t>
         </is>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="1" t="n">
         <v>6787224024000</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="1" t="n">
         <v>1519414377.43452</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="1" t="n">
         <v>6787224.024</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="1" t="n">
         <v>1519.41437743452</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="1" t="n">
         <v>6787.224024</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="H2" s="1" t="n">
         <v>1.51941437743452</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="I2" s="1" t="n">
         <v>113.1204004</v>
       </c>
-      <c r="J2" s="2" t="n">
+      <c r="J2" s="1" t="n">
         <v>0.025323572957242</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>v4</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" s="1" t="inlineStr">
         <is>
           <t>All sets</t>
         </is>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="1" t="n">
         <v>0.001</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="1" t="n">
         <v>0.001</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="1" t="n">
         <v>1e-06</v>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="H3" s="1" t="n">
         <v>1e-06</v>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="I3" s="1" t="n">
         <v>1.666666666666667e-08</v>
       </c>
-      <c r="J3" s="2" t="n">
+      <c r="J3" s="1" t="n">
         <v>1.666666666666667e-08</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>v3.5</t>
         </is>
       </c>
-      <c r="B4" s="2" t="inlineStr">
+      <c r="B4" s="1" t="inlineStr">
         <is>
           <t>00_#G03#</t>
         </is>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>1534230200</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>961297.1177944862</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>1534.2302</v>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>0.9612971177944862</v>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>1.5342302</v>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>0.0009612971177944863</v>
-      </c>
-      <c r="I4" s="2" t="n">
-        <v>0.02557050333333333</v>
-      </c>
-      <c r="J4" s="2" t="n">
-        <v>1.60216186299081e-05</v>
+      <c r="C4" s="1" t="n">
+        <v>2450747982900</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1535556380.263158</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>2450747.9829</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>1535.556380263158</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>2450.7479829</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>1.535556380263158</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>40.845799715</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>0.0255926063377193</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>v3.5</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B5" s="1" t="inlineStr">
         <is>
           <t>00_#G04#</t>
         </is>
       </c>
-      <c r="C5" s="2" t="n">
-        <v>1222486900</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>958813.2549019608</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>1222.4869</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>0.9588132549019608</v>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>1.2224869</v>
-      </c>
-      <c r="H5" s="2" t="n">
-        <v>0.0009588132549019608</v>
-      </c>
-      <c r="I5" s="2" t="n">
-        <v>0.02037478166666667</v>
-      </c>
-      <c r="J5" s="2" t="n">
-        <v>1.598022091503268e-05</v>
+      <c r="C5" s="1" t="n">
+        <v>1862922985700</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>1461116067.215686</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>1862922.9857</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>1461.116067215686</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>1862.9229857</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>1.461116067215686</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>31.04871642833333</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>0.02435193445359477</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>v3.5</t>
         </is>
       </c>
-      <c r="B6" s="2" t="inlineStr">
+      <c r="B6" s="1" t="inlineStr">
         <is>
           <t>01_#G03#</t>
         </is>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>1502864000</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>941644.1102756893</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>1502.864</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>0.9416441102756893</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>1.502864</v>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>0.0009416441102756892</v>
-      </c>
-      <c r="I6" s="2" t="n">
-        <v>0.02504773333333333</v>
-      </c>
-      <c r="J6" s="2" t="n">
-        <v>1.569406850459482e-05</v>
+      <c r="C6" s="1" t="n">
+        <v>2473553055400</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>1549845272.807018</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>2473553.0554</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>1549.845272807018</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>2473.5530554</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>1.549845272807018</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>41.22588425666667</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>0.02583075454678363</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="inlineStr">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>v4</t>
         </is>
       </c>
-      <c r="B7" s="2" t="inlineStr">
+      <c r="B7" s="1" t="inlineStr">
         <is>
           <t>00_#G03#</t>
         </is>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="1" t="n">
         <v>0.001</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="1" t="n">
         <v>0.001</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G7" s="1" t="n">
         <v>1e-06</v>
       </c>
-      <c r="H7" s="2" t="n">
+      <c r="H7" s="1" t="n">
         <v>1e-06</v>
       </c>
-      <c r="I7" s="2" t="n">
+      <c r="I7" s="1" t="n">
         <v>1.666666666666667e-08</v>
       </c>
-      <c r="J7" s="2" t="n">
+      <c r="J7" s="1" t="n">
         <v>1.666666666666667e-08</v>
       </c>
     </row>
@@ -2351,257 +2587,4 @@
   <autoFilter ref="A1:J1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="13.5" customWidth="1" min="1" max="1"/>
-    <col width="16.5" customWidth="1" min="2" max="2"/>
-    <col width="22.5" customWidth="1" min="3" max="3"/>
-    <col width="28.5" customWidth="1" min="4" max="4"/>
-    <col width="19.5" customWidth="1" min="5" max="5"/>
-    <col width="21" customWidth="1" min="6" max="6"/>
-    <col width="13.5" customWidth="1" min="7" max="7"/>
-    <col width="13.5" customWidth="1" min="8" max="8"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="8" t="inlineStr">
-        <is>
-          <t>Dataset</t>
-        </is>
-      </c>
-      <c r="B1" s="8" t="inlineStr">
-        <is>
-          <t>Run Count</t>
-        </is>
-      </c>
-      <c r="C1" s="8" t="inlineStr">
-        <is>
-          <t>Model Version</t>
-        </is>
-      </c>
-      <c r="D1" s="8" t="inlineStr">
-        <is>
-          <t>Threading Enabled</t>
-        </is>
-      </c>
-      <c r="E1" s="8" t="inlineStr">
-        <is>
-          <t>Nanoseconds</t>
-        </is>
-      </c>
-      <c r="F1" s="8" t="inlineStr">
-        <is>
-          <t>Milliseconds</t>
-        </is>
-      </c>
-      <c r="G1" s="8" t="inlineStr">
-        <is>
-          <t>Seconds</t>
-        </is>
-      </c>
-      <c r="H1" s="8" t="inlineStr">
-        <is>
-          <t>Minutes</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>#G02#</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>#G03#</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>#G04#</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>#G02#</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>#G03#</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>#G04#</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>gpt-3.5-turbo</t>
-        </is>
-      </c>
-      <c r="D7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:H1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>